<commit_message>
Union DGEA and stage 1 vs. normal
</commit_message>
<xml_diff>
--- a/New GSE details.xlsx
+++ b/New GSE details.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\[2021] iGEM\iGEM series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s2071467\Desktop\iGEM_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB93627-4A32-495B-8194-9D98DEE6DB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed" sheetId="1" r:id="rId1"/>
@@ -377,7 +376,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +449,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -1017,9 +1022,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1062,28 +1064,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1092,28 +1154,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1123,60 +1188,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1185,14 +1196,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1473,10 +1478,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GM66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G10" sqref="G10:K10"/>
     </sheetView>
   </sheetViews>
@@ -1498,73 +1503,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="74"/>
+      <c r="G1" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="71" t="s">
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="59" t="s">
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="71" t="s">
+      <c r="Q1" s="80"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="42"/>
-      <c r="U1" s="80" t="s">
+      <c r="T1" s="77"/>
+      <c r="U1" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="49" t="s">
+      <c r="V1" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="41" t="s">
+      <c r="W1" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="45" t="s">
+      <c r="X1" s="77"/>
+      <c r="Y1" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="49" t="s">
+      <c r="Z1" s="68" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="38" t="s">
+      <c r="A2" s="71"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="37" t="s">
         <v>61</v>
       </c>
       <c r="H2" s="2">
@@ -1576,10 +1581,10 @@
       <c r="J2" s="2">
         <v>3</v>
       </c>
-      <c r="K2" s="39">
+      <c r="K2" s="38">
         <v>4</v>
       </c>
-      <c r="L2" s="66">
+      <c r="L2" s="43">
         <v>1</v>
       </c>
       <c r="M2" s="2">
@@ -1588,98 +1593,98 @@
       <c r="N2" s="2">
         <v>3</v>
       </c>
-      <c r="O2" s="62">
+      <c r="O2" s="41">
         <v>4</v>
       </c>
-      <c r="P2" s="38">
+      <c r="P2" s="37">
         <v>0</v>
       </c>
       <c r="Q2" s="2">
         <v>1</v>
       </c>
-      <c r="R2" s="39">
+      <c r="R2" s="38">
         <v>2</v>
       </c>
-      <c r="S2" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="39" t="s">
+      <c r="S2" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="81"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="38" t="s">
+      <c r="U2" s="83"/>
+      <c r="V2" s="69"/>
+      <c r="W2" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="X2" s="39" t="s">
+      <c r="X2" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="50"/>
+      <c r="Y2" s="71"/>
+      <c r="Z2" s="69"/>
     </row>
     <row r="3" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="73">
+      <c r="B3" s="45">
         <v>132</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="30">
         <v>45220</v>
       </c>
       <c r="D3" s="15">
         <v>0</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <v>0</v>
       </c>
-      <c r="F3" s="63">
+      <c r="F3" s="42">
         <v>34</v>
       </c>
-      <c r="G3" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="67">
+      <c r="G3" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="44">
         <v>0</v>
       </c>
-      <c r="M3" s="34">
+      <c r="M3" s="33">
         <v>6</v>
       </c>
-      <c r="N3" s="34">
+      <c r="N3" s="33">
         <v>27</v>
       </c>
-      <c r="O3" s="63">
+      <c r="O3" s="42">
         <v>1</v>
       </c>
-      <c r="P3" s="30">
+      <c r="P3" s="29">
         <v>2</v>
       </c>
-      <c r="Q3" s="34">
+      <c r="Q3" s="33">
         <v>32</v>
       </c>
-      <c r="R3" s="31">
+      <c r="R3" s="30">
         <v>0</v>
       </c>
-      <c r="S3" s="67">
+      <c r="S3" s="44">
         <v>0</v>
       </c>
-      <c r="T3" s="31">
+      <c r="T3" s="30">
         <v>34</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="U3" s="35" t="s">
         <v>24</v>
       </c>
       <c r="V3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W3" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="X3" s="44" t="s">
+      <c r="W3" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="X3" s="54" t="s">
         <v>31</v>
       </c>
       <c r="Y3" s="15" t="s">
@@ -1690,76 +1695,76 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="73">
+      <c r="B4" s="45">
         <v>33</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="30">
         <v>54675</v>
       </c>
       <c r="D4" s="15">
         <v>465230</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <v>0</v>
       </c>
-      <c r="F4" s="63">
+      <c r="F4" s="42">
         <v>12</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="75">
+      <c r="H4" s="47">
         <v>1</v>
       </c>
-      <c r="I4" s="75">
+      <c r="I4" s="47">
         <v>3</v>
       </c>
-      <c r="J4" s="75">
+      <c r="J4" s="47">
         <v>7</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="40">
+      <c r="L4" s="39">
         <v>0</v>
       </c>
-      <c r="M4" s="40">
+      <c r="M4" s="39">
         <v>1</v>
       </c>
-      <c r="N4" s="40">
+      <c r="N4" s="39">
         <v>10</v>
       </c>
-      <c r="O4" s="40">
+      <c r="O4" s="39">
         <v>0</v>
       </c>
-      <c r="P4" s="35">
+      <c r="P4" s="34">
         <v>5</v>
       </c>
-      <c r="Q4" s="58">
+      <c r="Q4" s="40">
         <v>6</v>
       </c>
-      <c r="R4" s="36">
+      <c r="R4" s="35">
         <v>0</v>
       </c>
-      <c r="S4" s="67">
+      <c r="S4" s="44">
         <v>1</v>
       </c>
-      <c r="T4" s="31">
+      <c r="T4" s="30">
         <v>11</v>
       </c>
-      <c r="U4" s="36" t="s">
+      <c r="U4" s="35" t="s">
         <v>24</v>
       </c>
       <c r="V4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W4" s="30">
+      <c r="W4" s="29">
         <v>7</v>
       </c>
-      <c r="X4" s="31">
+      <c r="X4" s="30">
         <v>5</v>
       </c>
       <c r="Y4" s="15" t="s">
@@ -1770,72 +1775,72 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="29">
         <v>22</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>54675</v>
       </c>
       <c r="D5" s="15">
         <v>0</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>0</v>
       </c>
-      <c r="F5" s="63">
+      <c r="F5" s="42">
         <v>22</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="33">
         <v>0</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="33">
         <v>12</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="33">
         <v>10</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="30">
         <v>0</v>
       </c>
-      <c r="L5" s="67">
+      <c r="L5" s="44">
         <v>0</v>
       </c>
-      <c r="M5" s="34">
+      <c r="M5" s="33">
         <v>2</v>
       </c>
-      <c r="N5" s="34">
+      <c r="N5" s="33">
         <v>16</v>
       </c>
-      <c r="O5" s="63">
+      <c r="O5" s="42">
         <v>4</v>
       </c>
-      <c r="P5" s="30">
+      <c r="P5" s="29">
         <v>16</v>
       </c>
-      <c r="Q5" s="34">
+      <c r="Q5" s="33">
         <v>6</v>
       </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="67">
+      <c r="R5" s="30"/>
+      <c r="S5" s="44">
         <v>0</v>
       </c>
-      <c r="T5" s="31">
+      <c r="T5" s="30">
         <v>22</v>
       </c>
-      <c r="U5" s="36"/>
+      <c r="U5" s="35"/>
       <c r="V5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W5" s="30">
+      <c r="W5" s="29">
         <v>20</v>
       </c>
-      <c r="X5" s="31">
+      <c r="X5" s="30">
         <v>2</v>
       </c>
       <c r="Y5" s="15" t="s">
@@ -1846,62 +1851,62 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="29">
         <v>6</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="30">
         <v>62733</v>
       </c>
       <c r="D6" s="15">
         <v>0</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <v>3</v>
       </c>
-      <c r="F6" s="63">
+      <c r="F6" s="42">
         <v>3</v>
       </c>
-      <c r="G6" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P6" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T6" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U6" s="36"/>
+      <c r="G6" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="61"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" s="35"/>
       <c r="V6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W6" s="30">
+      <c r="W6" s="29">
         <v>4</v>
       </c>
-      <c r="X6" s="31">
+      <c r="X6" s="30">
         <v>2</v>
       </c>
       <c r="Y6" s="15" t="s">
@@ -1910,138 +1915,138 @@
       <c r="Z6" s="17"/>
     </row>
     <row r="7" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <v>78</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>54675</v>
       </c>
       <c r="D7" s="15">
         <v>0</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>39</v>
       </c>
-      <c r="F7" s="63">
+      <c r="F7" s="42">
         <v>39</v>
       </c>
-      <c r="G7" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P7" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R7" s="31"/>
-      <c r="S7" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T7" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U7" s="36"/>
+      <c r="G7" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" s="30"/>
+      <c r="S7" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T7" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" s="35"/>
       <c r="V7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W7" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X7" s="54"/>
+      <c r="W7" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X7" s="56"/>
       <c r="Y7" s="15" t="s">
         <v>31</v>
       </c>
       <c r="Z7" s="17"/>
     </row>
     <row r="8" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="30">
-        <v>24</v>
-      </c>
-      <c r="C8" s="31">
+      <c r="B8" s="29">
+        <v>24</v>
+      </c>
+      <c r="C8" s="30">
         <v>8152</v>
       </c>
       <c r="D8" s="15">
         <v>0</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <v>6</v>
       </c>
-      <c r="F8" s="63">
+      <c r="F8" s="42">
         <v>12</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="33">
         <v>0</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="33">
         <v>1</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="33">
         <v>5</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="30">
         <v>0</v>
       </c>
-      <c r="L8" s="67">
+      <c r="L8" s="44">
         <v>1</v>
       </c>
-      <c r="M8" s="34">
+      <c r="M8" s="33">
         <v>2</v>
       </c>
-      <c r="N8" s="34">
+      <c r="N8" s="33">
         <v>3</v>
       </c>
-      <c r="O8" s="63">
+      <c r="O8" s="42">
         <v>0</v>
       </c>
-      <c r="P8" s="30">
+      <c r="P8" s="29">
         <v>3</v>
       </c>
-      <c r="Q8" s="34">
+      <c r="Q8" s="33">
         <v>3</v>
       </c>
-      <c r="R8" s="31"/>
-      <c r="S8" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T8" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U8" s="36" t="s">
+      <c r="R8" s="30"/>
+      <c r="S8" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U8" s="35" t="s">
         <v>24</v>
       </c>
       <c r="V8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W8" s="30">
+      <c r="W8" s="29">
         <v>3</v>
       </c>
-      <c r="X8" s="31">
+      <c r="X8" s="30">
         <v>3</v>
       </c>
       <c r="Y8" s="15" t="s">
@@ -2052,64 +2057,64 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="29">
         <v>18</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>734</v>
       </c>
       <c r="D9" s="15">
         <v>0</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <v>9</v>
       </c>
-      <c r="F9" s="63">
+      <c r="F9" s="42">
         <v>9</v>
       </c>
-      <c r="G9" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N9" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O9" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P9" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R9" s="31"/>
-      <c r="S9" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T9" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U9" s="36"/>
+      <c r="G9" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P9" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" s="30"/>
+      <c r="S9" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T9" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U9" s="35"/>
       <c r="V9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W9" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X9" s="54" t="s">
+      <c r="W9" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X9" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y9" s="15" t="s">
@@ -2118,64 +2123,64 @@
       <c r="Z9" s="17"/>
     </row>
     <row r="10" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="30">
-        <v>31</v>
-      </c>
-      <c r="C10" s="31">
+      <c r="B10" s="29">
+        <v>31</v>
+      </c>
+      <c r="C10" s="30">
         <v>47231</v>
       </c>
       <c r="D10" s="15">
         <v>0</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <v>5</v>
       </c>
-      <c r="F10" s="63">
+      <c r="F10" s="42">
         <v>7</v>
       </c>
-      <c r="G10" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N10" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O10" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P10" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q10" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R10" s="31"/>
-      <c r="S10" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T10" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U10" s="36"/>
+      <c r="G10" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" s="30"/>
+      <c r="S10" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T10" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U10" s="35"/>
       <c r="V10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W10" s="30">
+      <c r="W10" s="29">
         <v>13</v>
       </c>
-      <c r="X10" s="31">
+      <c r="X10" s="30">
         <v>13</v>
       </c>
       <c r="Y10" s="15" t="s">
@@ -2186,64 +2191,64 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="29">
         <v>103</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>47306</v>
       </c>
       <c r="D11" s="15">
         <v>0</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <v>0</v>
       </c>
-      <c r="F11" s="63">
+      <c r="F11" s="42">
         <v>103</v>
       </c>
-      <c r="G11" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N11" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O11" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P11" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q11" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R11" s="31"/>
-      <c r="S11" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T11" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U11" s="36"/>
+      <c r="G11" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" s="30"/>
+      <c r="S11" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T11" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U11" s="35"/>
       <c r="V11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W11" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X11" s="54" t="s">
+      <c r="W11" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X11" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y11" s="15" t="s">
@@ -2252,64 +2257,64 @@
       <c r="Z11" s="17"/>
     </row>
     <row r="12" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="29">
         <v>26</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="30">
         <v>22011</v>
       </c>
       <c r="D12" s="15">
         <v>0</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <v>10</v>
       </c>
-      <c r="F12" s="63">
+      <c r="F12" s="42">
         <v>10</v>
       </c>
-      <c r="G12" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N12" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P12" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R12" s="31"/>
-      <c r="S12" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T12" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U12" s="36"/>
+      <c r="G12" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" s="30"/>
+      <c r="S12" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T12" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U12" s="35"/>
       <c r="V12" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W12" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X12" s="54" t="s">
+      <c r="W12" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X12" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y12" s="15" t="s">
@@ -2320,74 +2325,74 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="29">
         <v>130</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="30">
         <v>33297</v>
       </c>
       <c r="D13" s="15">
         <v>0</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <v>61</v>
       </c>
-      <c r="F13" s="63">
+      <c r="F13" s="42">
         <v>69</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="29">
         <v>1</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="33">
         <v>2</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="33">
         <v>35</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="33">
         <v>30</v>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="30">
         <v>1</v>
       </c>
-      <c r="L13" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N13" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O13" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P13" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q13" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R13" s="31"/>
-      <c r="S13" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T13" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U13" s="36" t="s">
+      <c r="L13" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O13" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" s="30"/>
+      <c r="S13" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T13" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U13" s="35" t="s">
         <v>24</v>
       </c>
       <c r="V13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W13" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X13" s="54" t="s">
+      <c r="W13" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X13" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y13" s="15" t="s">
@@ -2398,66 +2403,66 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="29">
         <v>131</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="30">
         <v>49386</v>
       </c>
       <c r="D14" s="15">
         <v>0</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <v>13</v>
       </c>
-      <c r="F14" s="63">
+      <c r="F14" s="42">
         <v>118</v>
       </c>
-      <c r="G14" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N14" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P14" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q14" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R14" s="31"/>
-      <c r="S14" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T14" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U14" s="36" t="s">
+      <c r="G14" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P14" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R14" s="30"/>
+      <c r="S14" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T14" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U14" s="35" t="s">
         <v>24</v>
       </c>
       <c r="V14" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W14" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X14" s="54" t="s">
+      <c r="W14" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X14" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y14" s="15" t="s">
@@ -2466,64 +2471,64 @@
       <c r="Z14" s="17"/>
     </row>
     <row r="15" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="29">
         <v>30</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="30">
         <v>70523</v>
       </c>
       <c r="D15" s="15">
         <v>0</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="29">
         <v>0</v>
       </c>
-      <c r="F15" s="63">
+      <c r="F15" s="42">
         <v>30</v>
       </c>
-      <c r="G15" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M15" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N15" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O15" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P15" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q15" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R15" s="31"/>
-      <c r="S15" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T15" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U15" s="36"/>
+      <c r="G15" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O15" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q15" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15" s="30"/>
+      <c r="S15" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T15" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U15" s="35"/>
       <c r="V15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W15" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X15" s="54" t="s">
+      <c r="W15" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X15" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y15" s="15" t="s">
@@ -2534,70 +2539,70 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="29">
         <v>35</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="30">
         <v>18708</v>
       </c>
       <c r="D16" s="15">
         <v>0</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="29">
         <v>7</v>
       </c>
-      <c r="F16" s="63">
+      <c r="F16" s="42">
         <v>28</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="34">
+      <c r="G16" s="29"/>
+      <c r="H16" s="33">
         <v>0</v>
       </c>
-      <c r="I16" s="34">
+      <c r="I16" s="33">
         <v>18</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="33">
         <v>10</v>
       </c>
-      <c r="K16" s="31">
+      <c r="K16" s="30">
         <v>0</v>
       </c>
-      <c r="L16" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M16" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N16" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O16" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P16" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q16" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R16" s="31"/>
-      <c r="S16" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T16" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U16" s="36"/>
+      <c r="L16" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N16" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O16" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P16" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q16" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R16" s="30"/>
+      <c r="S16" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T16" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U16" s="35"/>
       <c r="V16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W16" s="30">
+      <c r="W16" s="29">
         <v>12</v>
       </c>
-      <c r="X16" s="31">
+      <c r="X16" s="30">
         <v>16</v>
       </c>
       <c r="Y16" s="15" t="s">
@@ -2608,68 +2613,68 @@
       </c>
     </row>
     <row r="17" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="29">
         <v>100</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="30">
         <v>25526</v>
       </c>
       <c r="D17" s="15">
         <v>56</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="29">
         <v>50</v>
       </c>
-      <c r="F17" s="63">
+      <c r="F17" s="42">
         <v>50</v>
       </c>
-      <c r="G17" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="67">
+      <c r="G17" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="44">
         <v>2</v>
       </c>
-      <c r="M17" s="34">
+      <c r="M17" s="33">
         <v>9</v>
       </c>
-      <c r="N17" s="34">
+      <c r="N17" s="33">
         <v>34</v>
       </c>
-      <c r="O17" s="63">
+      <c r="O17" s="42">
         <v>5</v>
       </c>
-      <c r="P17" s="30">
-        <v>31</v>
-      </c>
-      <c r="Q17" s="34">
+      <c r="P17" s="29">
+        <v>31</v>
+      </c>
+      <c r="Q17" s="33">
         <v>19</v>
       </c>
-      <c r="R17" s="31">
+      <c r="R17" s="30">
         <v>0</v>
       </c>
-      <c r="S17" s="67">
+      <c r="S17" s="44">
         <v>3</v>
       </c>
-      <c r="T17" s="31">
+      <c r="T17" s="30">
         <v>47</v>
       </c>
-      <c r="U17" s="36" t="s">
+      <c r="U17" s="35" t="s">
         <v>24</v>
       </c>
       <c r="V17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W17" s="30">
+      <c r="W17" s="29">
         <v>58</v>
       </c>
-      <c r="X17" s="31">
+      <c r="X17" s="30">
         <v>42</v>
       </c>
       <c r="Y17" s="17" t="s">
@@ -2680,66 +2685,66 @@
       </c>
     </row>
     <row r="18" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="29">
         <v>30</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="30">
         <v>29373</v>
       </c>
       <c r="D18" s="15">
         <v>0</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="29">
         <v>0</v>
       </c>
-      <c r="F18" s="63">
+      <c r="F18" s="42">
         <v>30</v>
       </c>
-      <c r="G18" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M18" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N18" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O18" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P18" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q18" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R18" s="31"/>
-      <c r="S18" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T18" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U18" s="36" t="s">
+      <c r="G18" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M18" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O18" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P18" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q18" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R18" s="30"/>
+      <c r="S18" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T18" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U18" s="35" t="s">
         <v>24</v>
       </c>
       <c r="V18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W18" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X18" s="54" t="s">
+      <c r="W18" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X18" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y18" s="15" t="s">
@@ -2748,64 +2753,64 @@
       <c r="Z18" s="17"/>
     </row>
     <row r="19" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="29">
         <v>80</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="30">
         <v>49386</v>
       </c>
       <c r="D19" s="15">
         <v>0</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="29">
         <v>0</v>
       </c>
-      <c r="F19" s="63">
+      <c r="F19" s="42">
         <v>80</v>
       </c>
-      <c r="G19" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M19" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N19" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O19" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P19" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q19" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R19" s="31"/>
-      <c r="S19" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T19" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U19" s="36"/>
+      <c r="G19" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N19" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O19" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P19" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q19" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R19" s="30"/>
+      <c r="S19" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T19" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U19" s="35"/>
       <c r="V19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W19" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X19" s="54" t="s">
+      <c r="W19" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X19" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y19" s="15" t="s">
@@ -2814,64 +2819,64 @@
       <c r="Z19" s="17"/>
     </row>
     <row r="20" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="29">
         <v>20</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="30">
         <v>135750</v>
       </c>
       <c r="D20" s="15">
         <v>0</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="29">
         <v>0</v>
       </c>
-      <c r="F20" s="63">
+      <c r="F20" s="42">
         <v>20</v>
       </c>
-      <c r="G20" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M20" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N20" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O20" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P20" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q20" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R20" s="31"/>
-      <c r="S20" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T20" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U20" s="36"/>
+      <c r="G20" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M20" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O20" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P20" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R20" s="30"/>
+      <c r="S20" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T20" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U20" s="35"/>
       <c r="V20" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W20" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X20" s="54" t="s">
+      <c r="W20" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X20" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y20" s="15" t="s">
@@ -2882,66 +2887,66 @@
       </c>
     </row>
     <row r="21" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="29">
         <v>30</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="30">
         <v>41093</v>
       </c>
       <c r="D21" s="15">
         <v>0</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="29">
         <v>13</v>
       </c>
-      <c r="F21" s="63">
+      <c r="F21" s="42">
         <v>17</v>
       </c>
-      <c r="G21" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M21" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N21" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O21" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P21" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q21" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R21" s="31"/>
-      <c r="S21" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T21" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U21" s="36" t="s">
+      <c r="G21" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M21" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O21" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P21" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R21" s="30"/>
+      <c r="S21" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T21" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U21" s="35" t="s">
         <v>26</v>
       </c>
       <c r="V21" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W21" s="30">
+      <c r="W21" s="29">
         <v>15</v>
       </c>
-      <c r="X21" s="31">
+      <c r="X21" s="30">
         <v>15</v>
       </c>
       <c r="Y21" s="15" t="s">
@@ -2952,72 +2957,72 @@
       </c>
     </row>
     <row r="22" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="29">
         <v>8</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="30">
         <v>58201</v>
       </c>
       <c r="D22" s="15">
         <v>0</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="29">
         <v>0</v>
       </c>
-      <c r="F22" s="63">
+      <c r="F22" s="42">
         <v>8</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="H22" s="34">
+      <c r="H22" s="33">
         <v>3</v>
       </c>
-      <c r="I22" s="34">
+      <c r="I22" s="33">
         <v>3</v>
       </c>
-      <c r="J22" s="34">
+      <c r="J22" s="33">
         <v>2</v>
       </c>
-      <c r="K22" s="31">
+      <c r="K22" s="30">
         <v>0</v>
       </c>
-      <c r="L22" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="M22" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N22" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="O22" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="P22" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q22" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="R22" s="31"/>
-      <c r="S22" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="T22" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="U22" s="36"/>
+      <c r="L22" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O22" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="P22" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q22" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="R22" s="30"/>
+      <c r="S22" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="T22" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="U22" s="35"/>
       <c r="V22" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W22" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="X22" s="54" t="s">
+      <c r="W22" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="X22" s="56" t="s">
         <v>31</v>
       </c>
       <c r="Y22" s="15" t="s">
@@ -3028,13 +3033,13 @@
       </c>
     </row>
     <row r="23" spans="1:26" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B23" s="31">
         <v>82</v>
       </c>
-      <c r="C23" s="33">
+      <c r="C23" s="32">
         <v>70523</v>
       </c>
       <c r="D23" s="16">
@@ -3043,55 +3048,55 @@
       <c r="E23" s="19">
         <v>0</v>
       </c>
-      <c r="F23" s="74">
+      <c r="F23" s="46">
         <v>82</v>
       </c>
-      <c r="G23" s="77" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="M23" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="N23" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="O23" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="P23" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q23" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="R23" s="33"/>
-      <c r="S23" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="T23" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="U23" s="76"/>
+      <c r="G23" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="O23" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="P23" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q23" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="R23" s="32"/>
+      <c r="S23" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="T23" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="U23" s="48"/>
       <c r="V23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="W23" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="X23" s="57" t="s">
+      <c r="W23" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="X23" s="58" t="s">
         <v>31</v>
       </c>
       <c r="Y23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="Z23" s="84"/>
+      <c r="Z23" s="51"/>
     </row>
     <row r="24" spans="1:26" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="23"/>
@@ -3159,20 +3164,20 @@
       <c r="Z25" s="25"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A26" s="83" t="s">
+      <c r="A26" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="82">
+      <c r="B26" s="49">
         <f>SUM(B17:B18,B14,B13,B8,B4,B3)</f>
         <v>580</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
-      <c r="E26" s="82">
+      <c r="E26" s="49">
         <f>SUM(E18,E17,E14,E13,E8,E4,E3)</f>
         <v>130</v>
       </c>
-      <c r="F26" s="82">
+      <c r="F26" s="49">
         <f>SUM(F18,F17,F14,F13,F8,F4,F3)</f>
         <v>325</v>
       </c>
@@ -4319,26 +4324,61 @@
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="W19:X19"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
     <mergeCell ref="P20:Q20"/>
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="P22:Q22"/>
@@ -4355,61 +4395,26 @@
     <mergeCell ref="S15:T15"/>
     <mergeCell ref="S16:T16"/>
     <mergeCell ref="S18:T18"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="L19:O19"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="W19:X19"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="G11:K11"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4418,11 +4423,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FA529E-5DBB-47C9-8A42-F638DE72EEEB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HN350"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4477,31 +4482,31 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="26">
         <v>132</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="27" t="s">
+      <c r="F2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="26" t="s">
         <v>24</v>
       </c>
       <c r="J2" s="3" t="s">
@@ -4515,7 +4520,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="84" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9">
@@ -4661,7 +4666,7 @@
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="84" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="9">
@@ -4847,7 +4852,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="84" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="9">
@@ -4885,7 +4890,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="84" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="9">
@@ -4997,7 +5002,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="84" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="9">
@@ -5035,7 +5040,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="84" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="9">

</xml_diff>